<commit_message>
order scences and fix targets
</commit_message>
<xml_diff>
--- a/public/encuesta.xlsx
+++ b/public/encuesta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cynthia Vega\Documents\CMMEdu\RedFID\dash\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F869A409-79F5-4666-8EC8-1C89BB8F06FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BB6F73-A286-41DE-A1CE-B058D498562B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="720" windowWidth="18200" windowHeight="9390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2129" uniqueCount="1065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2129" uniqueCount="1068">
   <si>
     <t>ID</t>
   </si>
@@ -3313,6 +3313,15 @@
   </si>
   <si>
     <t xml:space="preserve">Carlos Rojas </t>
+  </si>
+  <si>
+    <t>Andrés Ortiz</t>
+  </si>
+  <si>
+    <t>Emilio Cariaga</t>
+  </si>
+  <si>
+    <t>Maximina Márquez Torres</t>
   </si>
 </sst>
 </file>
@@ -3971,8 +3980,8 @@
   <dimension ref="A1:AD1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <pane ySplit="2" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6300,7 +6309,7 @@
         <v>38</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>415</v>
+        <v>1065</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>416</v>
@@ -8509,7 +8518,7 @@
         <v>77</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>765</v>
+        <v>1066</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>766</v>
@@ -8749,7 +8758,7 @@
         <v>83</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>808</v>
+        <v>1067</v>
       </c>
       <c r="C59" s="14" t="s">
         <v>809</v>

</xml_diff>